<commit_message>
deleted some left over files
</commit_message>
<xml_diff>
--- a/misc/Retroadapter_USAParts.xlsx
+++ b/misc/Retroadapter_USAParts.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25915"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="16500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$H$14</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$H$19</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="60">
   <si>
     <t>Part</t>
   </si>
@@ -117,9 +122,6 @@
     <t>Price</t>
   </si>
   <si>
-    <t>70172352</t>
-  </si>
-  <si>
     <t>520-HCU150-20-4X</t>
   </si>
   <si>
@@ -155,6 +157,54 @@
   </si>
   <si>
     <t>Dsub gender changer cover 9 to 25 quick lock black, Northern Tech.</t>
+  </si>
+  <si>
+    <t>579-MCP1702-3302E/TO</t>
+  </si>
+  <si>
+    <t>MCP1702-3302E/TO</t>
+  </si>
+  <si>
+    <t>3.3 V LDO Voltage Regulators LDO w/ Low Quiescent (for N64/GC cable)</t>
+  </si>
+  <si>
+    <t>523-L77SDA15S</t>
+  </si>
+  <si>
+    <t>L77SDA15S</t>
+  </si>
+  <si>
+    <t>D-Sub Standard Connectors 15P FEMALE solder bucket</t>
+  </si>
+  <si>
+    <t>D-Sub Standard Connectors 9 POS. SOLDER FEMALE GOLD PLTD. CONTACTS</t>
+  </si>
+  <si>
+    <t>601-40-9709S</t>
+  </si>
+  <si>
+    <t>40-9709S</t>
+  </si>
+  <si>
+    <t>D-Sub Backshells HOOD PLASTIC 15 POS. STANDARD</t>
+  </si>
+  <si>
+    <t>601-40-9715H</t>
+  </si>
+  <si>
+    <t>40-9715H</t>
+  </si>
+  <si>
+    <t>601-40-9709H</t>
+  </si>
+  <si>
+    <t>40-9709H</t>
+  </si>
+  <si>
+    <t>D-Sub Backshells HOOD PLASTIC 9 POS. STANDARD</t>
+  </si>
+  <si>
+    <t>FOR THE CABLES (DB15: NeoGeo, Saturn, PSX, TurboGfx, Dual NES, Dual Atari; DB9: NES, SNES, N64/GC; two each)</t>
   </si>
 </sst>
 </file>
@@ -164,7 +214,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,6 +238,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -206,11 +264,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -235,21 +297,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="6">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -296,7 +358,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -331,7 +393,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -540,28 +602,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="58.265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.53125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.53125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.19921875" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.19921875" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.796875" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="58.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" s="5" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -572,22 +634,22 @@
         <v>29</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>31</v>
       </c>
       <c r="F1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -611,7 +673,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -636,7 +698,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -660,7 +722,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -684,7 +746,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -708,7 +770,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" s="1" customFormat="1">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -733,7 +795,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -758,7 +820,7 @@
         <v>3.93</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -783,7 +845,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -808,15 +870,15 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="E11" s="10">
         <v>0.53</v>
@@ -832,16 +894,16 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" s="1" customFormat="1">
       <c r="A12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E12" s="10">
         <v>4.8600000000000003</v>
@@ -857,12 +919,12 @@
         <v>4.8600000000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>32</v>
+        <v>43</v>
+      </c>
+      <c r="C13" s="17">
+        <v>70172352</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>30</v>
@@ -881,18 +943,165 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8">
+      <c r="A14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="13"/>
       <c r="G14" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H14" s="11">
         <f>SUM(H2:H13)</f>
         <v>13.390000000000002</v>
       </c>
     </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="10">
+        <v>0.52</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" s="1">
+        <v>2</v>
+      </c>
+      <c r="H16" s="9">
+        <f>E16*G16</f>
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="10">
+        <v>0.89</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="1">
+        <v>12</v>
+      </c>
+      <c r="H17" s="9">
+        <f>E17*G17</f>
+        <v>10.68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="10">
+        <v>0.61</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="1">
+        <v>6</v>
+      </c>
+      <c r="H18" s="9">
+        <f>E18*G18</f>
+        <v>3.66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="9">
+        <v>0.46</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19" s="15">
+        <v>12</v>
+      </c>
+      <c r="H19" s="9">
+        <f>E19*G19</f>
+        <v>5.5200000000000005</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" s="9">
+        <v>0.52</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="1">
+        <v>6</v>
+      </c>
+      <c r="H20" s="9">
+        <f>E20*G20</f>
+        <v>3.12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="G21" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H21" s="16">
+        <f>SUM(H16:H20)</f>
+        <v>24.02</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="87" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="87" orientation="landscape"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>